<commit_message>
Update the excel files and delete old unused csv files
</commit_message>
<xml_diff>
--- a/data/DB files - Excel/tblStudyFields.xlsx
+++ b/data/DB files - Excel/tblStudyFields.xlsx
@@ -8,7 +8,11 @@
   </bookViews>
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="tblStudyFields"/>
+    <sheet r:id="rId4" name="tblStudyFields1" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="tblStudyFields">'tblStudyFields1'!$A$1:$E$49</definedName>
+  </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
@@ -1563,4 +1567,1246 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Order</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Field Name</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Field Category</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>Field Type</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0">
+        <v>47</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>MPManagementTool</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Alternatives</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>Management alternatives evaluated in the study</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0">
+        <v>48</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>MPAlternativesEvaluated</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>Alternatives</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Types of alternatives evaluated</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0">
+        <v>40</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>ObjName</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>Objectives</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Text description of the objective</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0">
+        <v>41</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>ObjCategory</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>Objectives</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>The objective category (conservation, yield, economic, social)</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0">
+        <v>42</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>ObjDescription</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>Objectives</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Description of the objective</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0">
+        <v>43</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>ObjDirection</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>Objectives</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>The desired state of the objective</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0">
+        <v>44</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ObjType</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>Objectives</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>The type of objective.  E.g., strategic, process, fundamental, or means</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0">
+        <v>45</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>ObjScale</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>Objectives</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>The scale on which the objective is measures (natural, proxy, or constructed)</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0">
+        <v>46</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ObjMetric</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>Objectives</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>The units used to measure the objective</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0">
+        <v>19</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>ResultsAdopted</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>Did the MSE influence subsequent management?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0">
+        <v>20</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>Decision</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>If documented, the management procedure that was selected for implementation</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0">
+        <v>33</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Drivers</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>System drivers included in the operating model, e.g., climate change, environmental conditions, predation, species interactions, etc.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0">
+        <v>6</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>Latitude</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>Lat.</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>Center point of the geographic are the MSE applies to (latitude)</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="0">
+        <v>7</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>Longitude</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>Long.</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>Center point of the geographic are the MSE applies to (longitude)</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="0">
+        <v>2</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>Author</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>Names of the authors of the study</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="A17" s="0">
+        <v>3</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>YearPub</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>The year of publication</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="0">
+        <v>8</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>Species</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>Target species</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="A19" s="0">
+        <v>5</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>Geographic area the fishery occurs in</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="0">
+        <v>4</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>A short description of the study system.  For example, the species and it's location</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="A21" s="0">
+        <v>9</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>FullCitation</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>The full citation for the study</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="22">
+      <c r="A22" s="0">
+        <v>14</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ProcessExplicit</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>Was the decision process methodology documented clearly?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="23">
+      <c r="A23" s="0">
+        <v>15</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>RoleSpecification</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>Were roles assigned and documented?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="24">
+      <c r="A24" s="0">
+        <v>16</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>OpenMeetings</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>Were open meetings held?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="25">
+      <c r="A25" s="0">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ProblemDefinitionExplicit</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>Was a problem defintion completed and documented?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="26">
+      <c r="A26" s="0">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>ProblemDefinition</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t>A problem definition taken from the documentation (Reader interpretation)</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="27">
+      <c r="A27" s="0">
+        <v>25</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ObjectivesExplicit</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>Were objectives elicited and documented clearly?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="28">
+      <c r="A28" s="0">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>ObjElicitationMethod</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E28" s="0" t="inlineStr">
+        <is>
+          <t>If documented, how were objectives elicited?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="29">
+      <c r="A29" s="0">
+        <v>34</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>TradeOffsExplicit</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E29" s="0" t="inlineStr">
+        <is>
+          <t>Was a tradeoff analysis conducted and documented?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="30">
+      <c r="A30" s="0">
+        <v>35</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>TradeOffMethod_Exp</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E30" s="0" t="inlineStr">
+        <is>
+          <t>If explicitly documented, what form of tradeoff analysis occured?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="31">
+      <c r="A31" s="0">
+        <v>18</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>DecisionExplicit</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E31" s="0" t="inlineStr">
+        <is>
+          <t>Was the decision of the process documented?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="32">
+      <c r="A32" s="0">
+        <v>37</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E32" s="0" t="inlineStr">
+        <is>
+          <t>Additional notes and comments about the study</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="33">
+      <c r="A33" s="0">
+        <v>21</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>Leader</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E33" s="0" t="inlineStr">
+        <is>
+          <t>What organization initiated and directed the MSE?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="34">
+      <c r="A34" s="0">
+        <v>22</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>Participants</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E34" s="0" t="inlineStr">
+        <is>
+          <t>Who participated in the MSE process?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="35">
+      <c r="A35" s="0">
+        <v>26</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ObjElicitationSource_Exp</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E35" s="0" t="inlineStr">
+        <is>
+          <t>If explicitly documented, the groups from which objectives were elicited</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="36">
+      <c r="A36" s="0">
+        <v>30</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ProcedureElicitation_Exp</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E36" s="0" t="inlineStr">
+        <is>
+          <t>If explicitly documented, the groups from which alternative management procedures were elicited</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="37">
+      <c r="A37" s="0">
+        <v>32</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ConsequencePrediction</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E37" s="0" t="inlineStr">
+        <is>
+          <t>How were consequences predicted?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="38">
+      <c r="A38" s="0">
+        <v>17</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>OptimalAltExplicit</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E38" s="0" t="inlineStr">
+        <is>
+          <t>Was the best management procedure, aka optimal alternative, documented?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="39">
+      <c r="A39" s="0">
+        <v>29</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>AlternativesExplicit</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E39" s="0" t="inlineStr">
+        <is>
+          <t>Were alternatives elicited and documented clearly?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="40">
+      <c r="A40" s="0">
+        <v>36</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>TradeOffMethod_Sub</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>Decision Analysis</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E40" s="0" t="inlineStr">
+        <is>
+          <t>If not explicitly documented, what form of tradeoff analysis seems to have occured?</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="41">
+      <c r="A41" s="0">
+        <v>27</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>ObjElicitationSource_Sub</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E41" s="0" t="inlineStr">
+        <is>
+          <t>If not explicitly documented, the groups from which objectives were seemingly elicited</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="42">
+      <c r="A42" s="0">
+        <v>31</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ProcedureElicitation_Sub</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>Decision Process</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E42" s="0" t="inlineStr">
+        <is>
+          <t>If not explicitly documented, the groups from which alternative management procedures were seemingly elicited</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="43">
+      <c r="A43" s="0">
+        <v>1</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>DOI</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="E43" s="0" t="inlineStr">
+        <is>
+          <t>Digital Object Identifier (DOI)</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="44">
+      <c r="A44" s="0">
+        <v>10</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>AllAuthors</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t>A list of all of the authors of the publication, in last, first, initial.; format</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="45">
+      <c r="A45" s="0">
+        <v>11</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
+        <is>
+          <t>Title of the publication</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="46">
+      <c r="A46" s="0">
+        <v>12</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr">
+        <is>
+          <t>Journal in which the MSE study was published</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="47">
+      <c r="A47" s="0">
+        <v>13</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>poc</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="E47" s="0" t="inlineStr">
+        <is>
+          <t>Contact information (i.e., email address) for the publication's point of contact</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="48">
+      <c r="A48" s="0">
+        <v>38</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>RandomSample</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>Meta</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E48" s="0" t="inlineStr">
+        <is>
+          <t>Denotes whether the MSE was randomly sampled for review for inclusion in the publication, or not.</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="49">
+      <c r="A49" s="0">
+        <v>39</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>UseInPublication</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>Meta</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>Yes/No</t>
+        </is>
+      </c>
+      <c r="E49" s="0" t="inlineStr">
+        <is>
+          <t>Denotes whether the MSE was reviewed for inclusion in the publication, or not.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>